<commit_message>
Aggiornamento forecast DA 2025-10-29
</commit_message>
<xml_diff>
--- a/forecast_DE/df_DA_DE_2025-10-29.xlsx
+++ b/forecast_DE/df_DA_DE_2025-10-29.xlsx
@@ -414,13 +414,13 @@
         <v>45959</v>
       </c>
       <c r="B2">
-        <v>48209</v>
+        <v>48061</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>74830</v>
+        <v>37962</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -428,13 +428,13 @@
         <v>45959.04166666666</v>
       </c>
       <c r="B3">
-        <v>46506</v>
+        <v>46536</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>71141</v>
+        <v>36335</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -442,13 +442,13 @@
         <v>45959.08333333334</v>
       </c>
       <c r="B4">
-        <v>45581</v>
+        <v>45639</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>67951</v>
+        <v>35011</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -456,13 +456,13 @@
         <v>45959.125</v>
       </c>
       <c r="B5">
-        <v>45991</v>
+        <v>46060</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>65153</v>
+        <v>33667</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -470,13 +470,13 @@
         <v>45959.16666666666</v>
       </c>
       <c r="B6">
-        <v>47197</v>
+        <v>47295</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>62040</v>
+        <v>32154.5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -484,13 +484,13 @@
         <v>45959.20833333334</v>
       </c>
       <c r="B7">
-        <v>50557</v>
+        <v>50633</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>58784</v>
+        <v>30641</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -498,13 +498,13 @@
         <v>45959.25</v>
       </c>
       <c r="B8">
-        <v>57698</v>
+        <v>57774</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>55656</v>
+        <v>29213</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -512,13 +512,13 @@
         <v>45959.29166666666</v>
       </c>
       <c r="B9">
-        <v>62806</v>
+        <v>62858</v>
       </c>
       <c r="C9">
-        <v>4042</v>
+        <v>2071</v>
       </c>
       <c r="D9">
-        <v>52087</v>
+        <v>27597</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -526,13 +526,13 @@
         <v>45959.33333333334</v>
       </c>
       <c r="B10">
-        <v>65302</v>
+        <v>65338</v>
       </c>
       <c r="C10">
-        <v>15858</v>
+        <v>8050</v>
       </c>
       <c r="D10">
-        <v>48418</v>
+        <v>25805.5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -540,13 +540,13 @@
         <v>45959.375</v>
       </c>
       <c r="B11">
-        <v>66270</v>
+        <v>66158</v>
       </c>
       <c r="C11">
-        <v>30042</v>
+        <v>15549</v>
       </c>
       <c r="D11">
-        <v>45783</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -554,13 +554,13 @@
         <v>45959.41666666666</v>
       </c>
       <c r="B12">
-        <v>67041</v>
+        <v>67056</v>
       </c>
       <c r="C12">
-        <v>41086</v>
+        <v>21685</v>
       </c>
       <c r="D12">
-        <v>44430</v>
+        <v>22569.5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -568,13 +568,13 @@
         <v>45959.45833333334</v>
       </c>
       <c r="B13">
-        <v>67505</v>
+        <v>67572</v>
       </c>
       <c r="C13">
-        <v>45282</v>
+        <v>23653</v>
       </c>
       <c r="D13">
-        <v>43955</v>
+        <v>21864</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -582,13 +582,13 @@
         <v>45959.5</v>
       </c>
       <c r="B14">
-        <v>66928</v>
+        <v>67151</v>
       </c>
       <c r="C14">
-        <v>43372</v>
+        <v>22393</v>
       </c>
       <c r="D14">
-        <v>43072</v>
+        <v>21418.5</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -596,13 +596,13 @@
         <v>45959.54166666666</v>
       </c>
       <c r="B15">
-        <v>65640</v>
+        <v>65494</v>
       </c>
       <c r="C15">
-        <v>36284</v>
+        <v>18592</v>
       </c>
       <c r="D15">
-        <v>41807</v>
+        <v>20716</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -610,13 +610,13 @@
         <v>45959.58333333334</v>
       </c>
       <c r="B16">
-        <v>64090</v>
+        <v>63993</v>
       </c>
       <c r="C16">
-        <v>24992</v>
+        <v>12614</v>
       </c>
       <c r="D16">
-        <v>41420</v>
+        <v>19977.5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -624,13 +624,13 @@
         <v>45959.625</v>
       </c>
       <c r="B17">
-        <v>62661</v>
+        <v>62602</v>
       </c>
       <c r="C17">
-        <v>12298</v>
+        <v>6051</v>
       </c>
       <c r="D17">
-        <v>42346</v>
+        <v>20148</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -638,13 +638,13 @@
         <v>45959.66666666666</v>
       </c>
       <c r="B18">
-        <v>62374</v>
+        <v>62301</v>
       </c>
       <c r="C18">
-        <v>2956</v>
+        <v>1397</v>
       </c>
       <c r="D18">
-        <v>45695</v>
+        <v>21592</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -652,13 +652,13 @@
         <v>45959.70833333334</v>
       </c>
       <c r="B19">
-        <v>65458</v>
+        <v>65596</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>49973</v>
+        <v>23772</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -666,13 +666,13 @@
         <v>45959.75</v>
       </c>
       <c r="B20">
-        <v>65233</v>
+        <v>65385</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>52594</v>
+        <v>25521.5</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -680,13 +680,13 @@
         <v>45959.79166666666</v>
       </c>
       <c r="B21">
-        <v>63889</v>
+        <v>64085</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>53737</v>
+        <v>26407</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -694,13 +694,13 @@
         <v>45959.83333333334</v>
       </c>
       <c r="B22">
-        <v>60444</v>
+        <v>60694</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>53180</v>
+        <v>26297</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -708,13 +708,13 @@
         <v>45959.875</v>
       </c>
       <c r="B23">
-        <v>57046</v>
+        <v>57200</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>51514</v>
+        <v>25465.5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -722,13 +722,13 @@
         <v>45959.91666666666</v>
       </c>
       <c r="B24">
-        <v>53609</v>
+        <v>53743</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>50529</v>
+        <v>24760</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -736,13 +736,13 @@
         <v>45959.95833333334</v>
       </c>
       <c r="B25">
-        <v>49787</v>
+        <v>49913</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>50412</v>
+        <v>24705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>